<commit_message>
spare detection logic completed
</commit_message>
<xml_diff>
--- a/sampleFile.xlsx
+++ b/sampleFile.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C35127\Downloads\1-Teaching\ICS4U\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avih2\Documents\NetBeansProjects\SpareLink1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26418442-D5AC-40D8-99B0-3986EF42607B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15444" windowHeight="8988"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR_8340304443106797315" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="92">
   <si>
     <t>Student Number</t>
   </si>
@@ -265,9 +266,6 @@
   </si>
   <si>
     <t>1ELER2-03</t>
-  </si>
-  <si>
-    <t>BAT4M.-01</t>
   </si>
   <si>
     <t>ENG4U.-04</t>
@@ -303,7 +301,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1115,34 +1113,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17:AA18"/>
+      <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="5.77734375" customWidth="1"/>
-    <col min="13" max="20" width="5.77734375" customWidth="1"/>
-    <col min="21" max="21" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5.7109375" customWidth="1"/>
+    <col min="13" max="20" width="5.7109375" customWidth="1"/>
+    <col min="21" max="21" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1214,15 +1212,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123456789</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -1249,15 +1247,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>123456789</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -1284,15 +1282,15 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>123456789</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -1319,15 +1317,15 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>123456789</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1354,15 +1352,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>123456789</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -1389,15 +1387,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>123456789</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -1424,15 +1422,15 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>123456789</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -1459,15 +1457,15 @@
         <v>338</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>987654321</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>35</v>
@@ -1485,15 +1483,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>987654321</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>35</v>
@@ -1511,15 +1509,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>987654321</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>35</v>
@@ -1537,15 +1535,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>987654321</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>35</v>
@@ -1563,15 +1561,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>987654321</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>35</v>
@@ -1589,15 +1587,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>987654321</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>35</v>
@@ -1615,15 +1613,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>987654321</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>35</v>
@@ -1641,15 +1639,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>987654321</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>35</v>
@@ -1667,15 +1665,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>456789123</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
@@ -1697,15 +1695,15 @@
       </c>
       <c r="AA17" s="3"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>456789123</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
         <v>35</v>
@@ -1733,15 +1731,15 @@
       </c>
       <c r="AA18" s="3"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>456789123</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
         <v>35</v>
@@ -1759,7 +1757,7 @@
         <v>29</v>
       </c>
       <c r="W19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="X19" t="s">
         <v>76</v>
@@ -1768,15 +1766,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>456789123</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
         <v>35</v>
@@ -1803,15 +1801,15 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>456789123</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
@@ -1838,15 +1836,15 @@
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>456789123</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
         <v>35</v>
@@ -1864,7 +1862,7 @@
         <v>29</v>
       </c>
       <c r="W22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X22" t="s">
         <v>75</v>
@@ -1873,15 +1871,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>456789123</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
         <v>35</v>
@@ -1908,15 +1906,15 @@
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>456789123</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
         <v>35</v>
@@ -1943,15 +1941,15 @@
         <v>321</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>789123654</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>24</v>
@@ -1978,15 +1976,15 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>789123654</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>24</v>
@@ -2013,15 +2011,15 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>789123654</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>24</v>
@@ -2048,15 +2046,15 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>789123654</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>24</v>
@@ -2083,15 +2081,15 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>789123654</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>24</v>
@@ -2118,15 +2116,15 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>789123654</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>24</v>
@@ -2153,15 +2151,15 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>789123654</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>24</v>
@@ -2188,15 +2186,15 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>789123654</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>24</v>
@@ -2223,15 +2221,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>789123654</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>24</v>

</xml_diff>